<commit_message>
Latest Version 20:27 14-02-2025
</commit_message>
<xml_diff>
--- a/BEIN/Assets/Sectors.xlsx
+++ b/BEIN/Assets/Sectors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukhanyo\Desktop\Git Repo\BEIN\BEIN\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0E15313-54EE-489B-97D3-F53B25CAA72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0028CF-172E-4B1F-8749-79F06EA7817E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{128BD173-702D-4B87-B65B-69A6A2A79ABC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve"> Title</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>The landscaping sector focuses on designing, creating, and maintaining outdoor spaces to enhance their functionality, aesthetics, and environmental sustainability. It includes services like gardening, lawn care, tree planting, irrigation systems, and hardscaping, such as patios and walkways. This industry combines creativity with technical skills, playing a key role in residential, commercial, and public spaces.</t>
+  </si>
+  <si>
+    <t>Built Environment Engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The design, analysis, and development of human-made spaces where people live, work, and play. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The application of scientific and technical knowledge to design, analyze, and develop the human-made spaces where people live, work, and play. </t>
   </si>
 </sst>
 </file>
@@ -169,13 +178,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -511,27 +518,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6188F51A-5E5C-498C-957F-F46BFC2F7C38}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -632,6 +639,17 @@
       </c>
       <c r="C10" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>